<commit_message>
Update template import pegawai
</commit_message>
<xml_diff>
--- a/public/template/kepegawaian_template_pusdatren.xlsx
+++ b/public/template/kepegawaian_template_pusdatren.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Commit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5831EBA3-221A-4A32-8E96-6E2B67602FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E549B5DB-8099-4D8A-BB5D-5CEC94492F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
   <si>
     <t>Biodata*</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Nomor Telepon 2</t>
   </si>
   <si>
-    <t>E-Mail*</t>
-  </si>
-  <si>
     <t>Negara*</t>
   </si>
   <si>
@@ -108,54 +105,6 @@
     <t>Wafat*</t>
   </si>
   <si>
-    <t>Lembaga</t>
-  </si>
-  <si>
-    <t>Golongan</t>
-  </si>
-  <si>
-    <t>Jenis Jabatan</t>
-  </si>
-  <si>
-    <t>Tanggal Masuk</t>
-  </si>
-  <si>
-    <t>Kode Mapel</t>
-  </si>
-  <si>
-    <t>Nama Mapel</t>
-  </si>
-  <si>
-    <t>Keterangan Jabatan</t>
-  </si>
-  <si>
-    <t>Golongan Jabatan</t>
-  </si>
-  <si>
-    <t>Jabatan/Jenis Kontrak</t>
-  </si>
-  <si>
-    <t>Tanggal Mulai</t>
-  </si>
-  <si>
-    <t>Satuan Kerja</t>
-  </si>
-  <si>
-    <t>Jurusan</t>
-  </si>
-  <si>
-    <t>Kelas</t>
-  </si>
-  <si>
-    <t>Rombel</t>
-  </si>
-  <si>
-    <t>Jumlah Murid</t>
-  </si>
-  <si>
-    <t>Periode Awal</t>
-  </si>
-  <si>
     <t>No Passport</t>
   </si>
   <si>
@@ -163,13 +112,190 @@
   </si>
   <si>
     <t>Smartcard</t>
+  </si>
+  <si>
+    <t>WNI</t>
+  </si>
+  <si>
+    <t>3279123456784377</t>
+  </si>
+  <si>
+    <t>3504910473829473</t>
+  </si>
+  <si>
+    <t>Roby Trio Darma</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>1990-01-15</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>Universitas Contoh</t>
+  </si>
+  <si>
+    <t>08123456789</t>
+  </si>
+  <si>
+    <t>budi@example.com</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Jawa timur</t>
+  </si>
+  <si>
+    <t>Malang</t>
+  </si>
+  <si>
+    <t>Klojen</t>
+  </si>
+  <si>
+    <t>Jl. Contoh No.1</t>
+  </si>
+  <si>
+    <t>40115</t>
+  </si>
+  <si>
+    <t>Uji-Coba</t>
+  </si>
+  <si>
+    <t>Tidak</t>
+  </si>
+  <si>
+    <t>SMK Nurul Jadid</t>
+  </si>
+  <si>
+    <t>kontrak</t>
+  </si>
+  <si>
+    <t>2020-07-01</t>
+  </si>
+  <si>
+    <t>MCDK-009</t>
+  </si>
+  <si>
+    <t>Bahasa Indonesia</t>
+  </si>
+  <si>
+    <t>Grade A1</t>
+  </si>
+  <si>
+    <t>Staff IT</t>
+  </si>
+  <si>
+    <t>Keamanan</t>
+  </si>
+  <si>
+    <t>Kepala Keamanan</t>
+  </si>
+  <si>
+    <t>TKJ</t>
+  </si>
+  <si>
+    <t>12 Putri</t>
+  </si>
+  <si>
+    <t>Golongan I</t>
+  </si>
+  <si>
+    <t>Lembaga Pengajar</t>
+  </si>
+  <si>
+    <t>Golongan Pengajar</t>
+  </si>
+  <si>
+    <t>Jenis Jabatan Pengajar</t>
+  </si>
+  <si>
+    <t>Tanggal Masuk Pengajar</t>
+  </si>
+  <si>
+    <t>Kode Mapel Pengajar</t>
+  </si>
+  <si>
+    <t>Nama Mapel Pengajar</t>
+  </si>
+  <si>
+    <t>Lembaga Karyawan</t>
+  </si>
+  <si>
+    <t>Keterangan Jabatan Karyawan</t>
+  </si>
+  <si>
+    <t>Golongan Jabatan Karyawan</t>
+  </si>
+  <si>
+    <t>Jabatan/Jenis Kontrak Karyawan</t>
+  </si>
+  <si>
+    <t>Tanggal Mulai Karyawan</t>
+  </si>
+  <si>
+    <t>Satuan Kerja Pengurus</t>
+  </si>
+  <si>
+    <t>Keterangan Jabatan Pengurus</t>
+  </si>
+  <si>
+    <t>Golongan Jabatan Pengurus</t>
+  </si>
+  <si>
+    <t>Jabatan/Jenis Kontrak Pengurus</t>
+  </si>
+  <si>
+    <t>Tanggal Mulai Pengurus</t>
+  </si>
+  <si>
+    <t>Lembaga Wali Kelas</t>
+  </si>
+  <si>
+    <t>Jurusan Wali Kelas</t>
+  </si>
+  <si>
+    <t>Kelas Wali Kelas</t>
+  </si>
+  <si>
+    <t>Rombel Wali Kelas</t>
+  </si>
+  <si>
+    <t>Jumlah Murid Wali Kelas</t>
+  </si>
+  <si>
+    <t>Periode Awal Wali Kelas</t>
+  </si>
+  <si>
+    <t>Email*</t>
+  </si>
+  <si>
+    <t>WNA</t>
+  </si>
+  <si>
+    <t>Sanzy</t>
+  </si>
+  <si>
+    <t>bud@example.com</t>
+  </si>
+  <si>
+    <t>N-1234</t>
+  </si>
+  <si>
+    <t>N-12347</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,8 +311,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,8 +333,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -223,11 +363,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -240,14 +392,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,86 +687,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AP11" sqref="AP11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="10" max="10" width="27.90625" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
+    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="7" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7" t="s">
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7" t="s">
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7"/>
-      <c r="AL1" s="7"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
       <c r="AM1" s="5"/>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AO1" s="7"/>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="7"/>
-      <c r="AR1" s="7"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
     </row>
     <row r="2" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
@@ -635,97 +811,351 @@
         <v>15</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="W2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="U3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO3" s="10">
+        <v>12</v>
+      </c>
+      <c r="AP3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ3" s="10">
+        <v>32</v>
+      </c>
+      <c r="AR3" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD2" s="3" t="s">
+      <c r="C4" s="7"/>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="H4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="I4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="J4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="K4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK2" s="3" t="s">
+      <c r="L4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="V4" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO4" s="10">
+        <v>12</v>
+      </c>
+      <c r="AP4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ4" s="10">
         <v>32</v>
       </c>
-      <c r="AL2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>39</v>
+      <c r="AR4" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -736,6 +1166,10 @@
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AN1:AR1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1" xr:uid="{D1909B63-0BCD-4780-986D-EA35038948C8}"/>
+    <hyperlink ref="N4" r:id="rId2" xr:uid="{3F9477F9-465D-4010-A53B-61734462B257}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>